<commit_message>
implementing latin hypercube sampling
</commit_message>
<xml_diff>
--- a/parameters/Task10_Param_Ranges.xlsx
+++ b/parameters/Task10_Param_Ranges.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steinanf/git/TMDD_EndogenousLigand/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB9EC61-7E53-AA46-82C4-B5E56560B461}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B5A739-2C59-D04A-9E77-1385E30A7782}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5660" yWindow="460" windowWidth="26840" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="460" windowWidth="26840" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Task05_Param_Summary" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="mpk2nmol">Task05_Param_Summary!$G$2</definedName>
-    <definedName name="Ms2nMd">Task05_Param_Summary!$G$14</definedName>
-    <definedName name="nmol2mpk">Task05_Param_Summary!$H$5</definedName>
+    <definedName name="mpk2nmol">Task05_Param_Summary!$H$13</definedName>
+    <definedName name="Ms2nMd">Task05_Param_Summary!$H$24</definedName>
+    <definedName name="nmol2mpk">Task05_Param_Summary!$I$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>k12</t>
+  </si>
+  <si>
+    <t>k21</t>
+  </si>
+  <si>
+    <t>keD</t>
+  </si>
   <si>
     <t>keT</t>
   </si>
@@ -47,6 +59,15 @@
     <t>keTL</t>
   </si>
   <si>
+    <t>Vm</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Km</t>
+  </si>
+  <si>
     <t>kon_DT</t>
   </si>
   <si>
@@ -122,12 +143,6 @@
     <t>dose</t>
   </si>
   <si>
-    <t>Conversion</t>
-  </si>
-  <si>
-    <t>mpk2nmol</t>
-  </si>
-  <si>
     <t>Reasonable range</t>
   </si>
   <si>
@@ -137,9 +152,6 @@
     <t>mg/kg</t>
   </si>
   <si>
-    <t>dose*mpk2nmol/(CL*tau)</t>
-  </si>
-  <si>
     <t>Median of Fig 5-18 from rowland and tozer.  Using dose rather than CL to explore</t>
   </si>
   <si>
@@ -150,6 +162,36 @@
   </si>
   <si>
     <t>Ms2nMd</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>CL = dose*mpk2nmol/(CL*tau)</t>
+  </si>
+  <si>
+    <t>Conversion: mpk2nmol</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>ka</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>nmol/d</t>
   </si>
 </sst>
 </file>
@@ -636,7 +678,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -657,6 +699,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -704,7 +749,16 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -768,14 +822,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25644456-42A2-3D4A-B14C-1737E6FCE0B1}" name="Table1" displayName="Table1" ref="A1:E15" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:E15" xr:uid="{33B61081-9DA4-A642-AE1F-70B00DEEC51F}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C8277EEB-8EE6-714C-B0D8-AA771A54F03E}" name="Parameter" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{CB33B989-EEDA-F24C-A340-C67DA904A869}" name="min" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25644456-42A2-3D4A-B14C-1737E6FCE0B1}" name="Table1" displayName="Table1" ref="A1:F25" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+  <autoFilter ref="A1:F25" xr:uid="{33B61081-9DA4-A642-AE1F-70B00DEEC51F}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{C8277EEB-8EE6-714C-B0D8-AA771A54F03E}" name="Parameter" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{CB33B989-EEDA-F24C-A340-C67DA904A869}" name="min" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{E0D84941-0EC1-B34A-87D8-EAFEA5BC7DFF}" name="max"/>
-    <tableColumn id="4" xr3:uid="{F264790B-6115-634D-BB49-151AB79FEF95}" name="units" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{CDC9DF67-3B1F-2C47-BF7C-1E440D4775CB}" name="Reference" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{F264790B-6115-634D-BB49-151AB79FEF95}" name="units" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{2ED0BCD4-C17C-4941-ACD4-22AB538EA128}" name="fixed" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{CDC9DF67-3B1F-2C47-BF7C-1E440D4775CB}" name="Reference" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1078,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="237" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="237" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1090,301 +1145,518 @@
     <col min="2" max="2" width="8" style="4" customWidth="1"/>
     <col min="3" max="3" width="10.1640625" style="4" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="33.83203125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="10.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="33.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="4">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="4">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4">
+        <f>B4/B6</f>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="C8" s="4">
+        <f>C4/C6</f>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5">
+        <f>B5/B6</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C9" s="5">
+        <f>C5/C6</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5">
+        <f>B5/B7</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C10" s="5">
+        <f>C5/C7</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="10">
+        <v>1</v>
+      </c>
+      <c r="C12" s="10">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="5">
+        <f>B15*mpk2nmol/(B4*B14)</f>
+        <v>0.92592592592592615</v>
+      </c>
+      <c r="C13" s="6">
+        <f>C15*mpk2nmol/(C4*C14)</f>
+        <v>9259.2592592592609</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="5">
-        <f>B5*mpk2nmol/(B3*B4)</f>
-        <v>0.92592592592592615</v>
-      </c>
-      <c r="C2" s="6">
-        <f>C5*mpk2nmol/(C3*C4)</f>
-        <v>9259.2592592592609</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="F13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="1">
         <f>70*0.001/150000*1000000000</f>
         <v>466.66666666666674</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4">
-        <v>2.4</v>
-      </c>
-      <c r="C3" s="4">
-        <v>2.4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="4">
+        <v>21</v>
+      </c>
+      <c r="C14" s="4">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="4">
-        <v>21</v>
-      </c>
-      <c r="C4" s="4">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="B15" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="C5" s="4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7">
+        <v>1E-4</v>
+      </c>
+      <c r="C16" s="4">
         <v>1000</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="7">
+      <c r="D16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="7">
         <v>1E-4</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C17" s="4">
         <v>1000</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="7">
-        <v>1E-4</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1000</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="D17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="4">
         <v>0</v>
       </c>
-      <c r="B8" s="4">
+      <c r="F17" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="4">
         <f>1*24*60</f>
         <v>1440</v>
       </c>
-      <c r="C8" s="8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="4">
+      <c r="C18" s="8">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="4">
         <f>1*24*60</f>
         <v>1440</v>
       </c>
-      <c r="C9" s="8">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="4">
+      <c r="C19" s="8">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="4">
         <f>1*24*60</f>
         <v>1440</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C20" s="8">
         <f>1/7/4</f>
         <v>3.5714285714285712E-2</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="4">
+      <c r="D20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="4">
         <f>1*24*60</f>
         <v>1440</v>
       </c>
-      <c r="C11" s="8">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="C21" s="8">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="4">
+      <c r="B22" s="4">
         <v>1E-3</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C22" s="4">
         <v>1000</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="C13" s="4">
-        <v>1000</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="4">
-        <v>1</v>
-      </c>
-      <c r="C14" s="9">
+      <c r="B24" s="4">
+        <v>1</v>
+      </c>
+      <c r="C24" s="9">
         <v>10000</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="1">
+      <c r="D24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H24" s="1">
         <f>1/1000000000*24*60*60</f>
         <v>8.6400000000000013E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="4">
-        <v>1</v>
-      </c>
-      <c r="C15" s="9">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1</v>
+      </c>
+      <c r="C25" s="9">
         <v>10000</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C18" s="7"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C20" s="7"/>
+      <c r="D25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C28" s="7"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C30" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>